<commit_message>
Probability higher revision in costs and utilities
</commit_message>
<xml_diff>
--- a/data/KNIPS Main input data.xlsx
+++ b/data/KNIPS Main input data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/KNIPS/code/KNIPS-Semi-Markov/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14D17B6D-6310-4769-AAB7-AB063EDB7AF1}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D914D825-2D0E-4431-9F1F-BBFB2BC56B01}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="implant_costs" sheetId="1" r:id="rId1"/>
     <sheet name="other_costs" sheetId="2" r:id="rId2"/>
     <sheet name="utilities" sheetId="3" r:id="rId3"/>
-    <sheet name="uk_lifetables" sheetId="9" r:id="rId4"/>
-    <sheet name="rcs_second_revision_mean" sheetId="7" r:id="rId5"/>
-    <sheet name="ln_bhknots_second_revision" sheetId="8" r:id="rId6"/>
-    <sheet name="second_revision_covariance" sheetId="4" r:id="rId7"/>
+    <sheet name="other_rates" sheetId="10" r:id="rId4"/>
+    <sheet name="uk_lifetables" sheetId="9" r:id="rId5"/>
+    <sheet name="rcs_second_revision_mean" sheetId="7" r:id="rId6"/>
+    <sheet name="ln_bhknots_second_revision" sheetId="8" r:id="rId7"/>
+    <sheet name="second_revision_covariance" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>xb:</t>
   </si>
@@ -214,6 +215,15 @@
   </si>
   <si>
     <t>bound2</t>
+  </si>
+  <si>
+    <t>lograte_higher_revision_mean</t>
+  </si>
+  <si>
+    <t>lograte_higher_revision_se</t>
+  </si>
+  <si>
+    <t>Inverse variance meta-analysis of log rates 3rd,.., 8th revision from NJR estimates</t>
   </si>
 </sst>
 </file>
@@ -866,6 +876,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C755A-13C4-4332-94A2-1BC44FBE376A}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="25.20703125" customWidth="1"/>
+    <col min="2" max="2" width="17.89453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>-3.0733869999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>1.4991249999999999E-4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95C669A-5DF0-42B7-80AB-F72C264CEB49}">
   <dimension ref="A1:C102"/>
   <sheetViews>
@@ -2002,7 +2065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AFC646-3F33-4729-B1CE-BFC81EDA6C3D}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2051,11 +2114,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084104AD-8338-457A-9F1C-E200B1ECC985}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2094,7 +2157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D6DFB3-35E3-4A4B-92F1-0C6BBB7EDA89}">
   <dimension ref="A1:I10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Corrected Excel format to align with readxl package
</commit_message>
<xml_diff>
--- a/data/KNIPS Main input data.xlsx
+++ b/data/KNIPS Main input data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4898e5cc837f6cd5/Documents/Bristol/KNIPS/code/KNIPS-Semi-Markov/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD842D8E-80C6-4607-86D6-0F1829FDE5AF}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="11_AD4DB114E441178AC67DF42F3E16E7F2683EDF1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A642850-628D-4E43-9908-234893C67D9D}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,13 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="87">
-  <si>
-    <t>xb:</t>
-  </si>
-  <si>
-    <t>dxb:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>yrs_to_1st~v</t>
   </si>
@@ -237,12 +231,6 @@
     <t>pre primary</t>
   </si>
   <si>
-    <t>ll</t>
-  </si>
-  <si>
-    <t>UL</t>
-  </si>
-  <si>
     <t>pre revision</t>
   </si>
   <si>
@@ -304,13 +292,64 @@
   </si>
   <si>
     <t>rerevision_prop_dead</t>
+  </si>
+  <si>
+    <t>pre primary ll</t>
+  </si>
+  <si>
+    <t>pre primary UL</t>
+  </si>
+  <si>
+    <t>6 months after primary ll</t>
+  </si>
+  <si>
+    <t>6 months after primary UL</t>
+  </si>
+  <si>
+    <t>pre revision ll</t>
+  </si>
+  <si>
+    <t>pre revision UL</t>
+  </si>
+  <si>
+    <t>6 months after revision ll</t>
+  </si>
+  <si>
+    <t>6 months after revision UL</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>xb1</t>
+  </si>
+  <si>
+    <t>xb2</t>
+  </si>
+  <si>
+    <t>xb3</t>
+  </si>
+  <si>
+    <t>xb4</t>
+  </si>
+  <si>
+    <t>xb5</t>
+  </si>
+  <si>
+    <t>xb6</t>
+  </si>
+  <si>
+    <t>xb7</t>
+  </si>
+  <si>
+    <t>xb8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +380,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -689,21 +734,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -719,7 +764,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>600</v>
@@ -735,7 +780,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>700</v>
@@ -751,7 +796,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>800</v>
@@ -767,7 +812,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>900</v>
@@ -783,7 +828,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -799,7 +844,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>500</v>
@@ -815,7 +860,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>600</v>
@@ -831,7 +876,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>700</v>
@@ -847,7 +892,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>800</v>
@@ -863,7 +908,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>900</v>
@@ -879,7 +924,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>500</v>
@@ -910,31 +955,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -945,7 +990,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D2" s="10">
         <v>100000</v>
@@ -974,7 +1019,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D3" s="10">
         <v>100000</v>
@@ -1006,7 +1051,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="10">
         <v>100000</v>
@@ -1038,7 +1083,7 @@
         <v>85</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5" s="10">
         <v>100000</v>
@@ -1067,10 +1112,10 @@
         <v>85</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="10">
         <v>100000</v>
@@ -1102,7 +1147,7 @@
         <v>55</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="10">
         <v>100000</v>
@@ -1134,7 +1179,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D8" s="10">
         <v>100000</v>
@@ -1166,7 +1211,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" s="10">
         <v>100000</v>
@@ -1198,7 +1243,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D10" s="10">
         <v>100000</v>
@@ -1227,10 +1272,10 @@
         <v>85</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D11" s="10">
         <v>100000</v>
@@ -1271,35 +1316,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>5000</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3">
         <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1322,15 +1367,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>-0.1</v>
@@ -1338,7 +1383,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
@@ -1346,7 +1391,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0.85</v>
@@ -1354,7 +1399,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>0.75</v>
@@ -1362,7 +1407,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>0.65</v>
@@ -1370,7 +1415,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>0.01</v>
@@ -1378,7 +1423,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>0.01</v>
@@ -1386,7 +1431,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>0.01</v>
@@ -1402,74 +1447,74 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="I1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="U1" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -1480,7 +1525,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1521,7 +1566,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1562,7 +1607,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1603,7 +1648,7 @@
         <v>85</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1641,10 +1686,10 @@
         <v>85</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -1685,7 +1730,7 @@
         <v>55</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1726,7 +1771,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1767,7 +1812,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1808,7 +1853,7 @@
         <v>85</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1846,10 +1891,10 @@
         <v>85</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1904,18 +1949,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>-4</v>
@@ -1923,7 +1968,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>1E-4</v>
@@ -1947,13 +1992,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -3084,19 +3129,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -3133,16 +3178,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -3169,66 +3214,69 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1.0000000000000001E-5</v>
@@ -3236,7 +3284,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1">
         <v>-9.9999999999999995E-7</v>
@@ -3247,7 +3295,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>-9.9999999999999995E-7</v>
@@ -3261,7 +3309,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>9.9999999999999995E-7</v>
@@ -3278,7 +3326,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>-9.9999999999999995E-7</v>
@@ -3298,7 +3346,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>9.9999999999999995E-7</v>
@@ -3321,7 +3369,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
         <v>-9.9999999999999995E-7</v>
@@ -3347,7 +3395,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>9.9999999999999995E-7</v>
@@ -3375,6 +3423,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>